<commit_message>
updated gitignore and deploy files
</commit_message>
<xml_diff>
--- a/data/excel/tutorial_home.xlsx
+++ b/data/excel/tutorial_home.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASHMI\DroidBiz\v3\DroidBizNextjs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422C36F5-BEBB-46B6-A36D-3C0021ACCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017375DF-1792-4108-BE9E-61739A897EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>kotlin</t>
-  </si>
-  <si>
-    <t>kotlin-new</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,24 +609,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>

</xml_diff>